<commit_message>
AutoDS Enrichissement E/S données + cohérence jeux de tests
</commit_message>
<xml_diff>
--- a/autods/refin/ACDC2019-Naturalist-SpecsAnalyses.xlsx
+++ b/autods/refin/ACDC2019-Naturalist-SpecsAnalyses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\jpm-perso\AutoDS\refin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\perso\autods\refin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88434B9D-288A-4DF5-A4FF-E7235D087EE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6127F217-1120-4967-9A55-3F5963AC924E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13968" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13968" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Echant1_impl" sheetId="1" r:id="rId1"/>
@@ -83,16 +83,16 @@
     <t>Lanius collurio</t>
   </si>
   <si>
-    <t>Espece</t>
-  </si>
-  <si>
-    <t>Duree</t>
-  </si>
-  <si>
-    <t>FonctionCle</t>
-  </si>
-  <si>
-    <t>SerieAjust</t>
+    <t>Durée</t>
+  </si>
+  <si>
+    <t>Espèce</t>
+  </si>
+  <si>
+    <t>SérieAjust</t>
+  </si>
+  <si>
+    <t>FonctionClé</t>
   </si>
 </sst>
 </file>
@@ -457,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,7 +471,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -480,7 +480,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -523,7 +523,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,7 +536,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -545,7 +545,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -581,7 +581,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,10 +592,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -621,7 +621,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,7 +636,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -645,7 +645,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>13</v>
@@ -1041,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474A5133-9B74-4D19-823B-523AF343B54A}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1057,7 +1057,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1066,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
AutoDS Cohérence jeux données / specs analyses, cosmétique, deprecation warning df.append
</commit_message>
<xml_diff>
--- a/autods/refin/ACDC2019-Naturalist-SpecsAnalyses.xlsx
+++ b/autods/refin/ACDC2019-Naturalist-SpecsAnalyses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\perso\autods\refin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6127F217-1120-4967-9A55-3F5963AC924E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1F767B-DE06-43DB-B27A-E03327BADD8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13968" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,18 +41,12 @@
     <t>m</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>Turdus merula</t>
   </si>
   <si>
     <t>m+a</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>Alauda arvensis</t>
   </si>
   <si>
@@ -93,6 +87,12 @@
   </si>
   <si>
     <t>FonctionClé</t>
+  </si>
+  <si>
+    <t>5mn</t>
+  </si>
+  <si>
+    <t>10mn</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,7 +471,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -480,7 +480,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -494,23 +494,23 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -523,7 +523,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,7 +536,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -545,29 +545,29 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -581,7 +581,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,23 +592,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -621,7 +621,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,7 +636,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -645,16 +645,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -668,7 +668,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -682,7 +682,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -699,7 +699,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F4">
         <v>280</v>
@@ -716,7 +716,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -736,7 +736,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>20</v>
@@ -759,7 +759,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -773,7 +773,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E8">
         <v>10</v>
@@ -790,7 +790,7 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F9">
         <v>280</v>
@@ -807,7 +807,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E10">
         <v>15</v>
@@ -827,7 +827,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E11">
         <v>20</v>
@@ -847,10 +847,10 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -861,10 +861,10 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -878,10 +878,10 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F14">
         <v>280</v>
@@ -895,10 +895,10 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E15">
         <v>15</v>
@@ -915,10 +915,10 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E16">
         <v>20</v>
@@ -932,7 +932,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
@@ -941,12 +941,12 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -955,7 +955,7 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F18">
         <v>450</v>
@@ -963,7 +963,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
@@ -972,7 +972,7 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F19">
         <v>500</v>
@@ -983,7 +983,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -992,12 +992,12 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
@@ -1006,7 +1006,7 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F21">
         <v>500</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
@@ -1023,7 +1023,7 @@
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F22">
         <v>600</v>
@@ -1042,7 +1042,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D7" sqref="D7:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1057,7 +1057,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1066,44 +1066,44 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -1111,16 +1111,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F4">
         <v>280</v>
@@ -1128,16 +1128,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -1151,30 +1151,30 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E7">
         <v>10</v>
@@ -1182,16 +1182,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F8">
         <v>350</v>
@@ -1199,16 +1199,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E9">
         <v>15</v>
@@ -1219,30 +1219,30 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F11">
         <v>300</v>
@@ -1250,16 +1250,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E12">
         <v>20</v>

</xml_diff>